<commit_message>
done with lab 3
</commit_message>
<xml_diff>
--- a/diff amp.xlsx
+++ b/diff amp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>f</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>Sunil data</t>
+  </si>
+  <si>
+    <t>Differential Amp Characteristics</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>Gain(dB)</t>
   </si>
 </sst>
 </file>
@@ -2090,6 +2099,660 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1848117296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$134:$A$145</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1700000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1800000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1900000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$134:$B$145</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.53739999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.72419999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.9381999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.1581000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.3837000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.8532999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-3.0979999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.8763999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.1521999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-45ED-4CFB-A056-05B1D1B078FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1404578847"/>
+        <c:axId val="1404568447"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1404578847"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1404568447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1404568447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.2"/>
+          <c:min val="-4.4000000000000004"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1404578847"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$150:$A$160</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>160000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$150:$B$160</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.645399999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.062000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.902000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.112400000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BC1D-4749-994B-C4EB624A141E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1400117423"/>
+        <c:axId val="1400117839"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1400117423"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1400117839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1400117839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="20.100000000000001"/>
+          <c:min val="13.9"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1400117423"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2378,6 +3041,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4959,6 +5702,1038 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5656,6 +7431,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>15874</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>51858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>735541</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>37041</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>189440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>756708</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>117474</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5925,10 +7760,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G128"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="90" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="90" workbookViewId="0">
+      <selection activeCell="I132" sqref="I132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7250,6 +9085,219 @@
         <v>259.2</v>
       </c>
     </row>
+    <row r="132" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>100</v>
+      </c>
+      <c r="B134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>500</v>
+      </c>
+      <c r="B135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B137" s="1">
+        <v>-0.53739999999999999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B138" s="1">
+        <v>-0.72419999999999995</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B139" s="1">
+        <v>-1.9381999999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="B140" s="1">
+        <v>-2.1581000000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>1600000</v>
+      </c>
+      <c r="B141" s="1">
+        <v>-2.3837000000000002</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>1700000</v>
+      </c>
+      <c r="B142" s="1">
+        <v>-2.8532999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>1800000</v>
+      </c>
+      <c r="B143" s="1">
+        <v>-3.0979999999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>1900000</v>
+      </c>
+      <c r="B144" s="1">
+        <v>-3.8763999999999998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="B145" s="1">
+        <v>-4.1521999999999997</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+    </row>
+    <row r="149" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>0</v>
+      </c>
+      <c r="B149" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>100</v>
+      </c>
+      <c r="B150" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>500</v>
+      </c>
+      <c r="B151" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B152" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B153" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B154" s="1">
+        <v>19.645399999999999</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>60000</v>
+      </c>
+      <c r="B155" s="1">
+        <v>18.690000000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B156" s="1">
+        <v>18.062000000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>104000</v>
+      </c>
+      <c r="B157" s="1">
+        <v>16.902000000000001</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>120000</v>
+      </c>
+      <c r="B158" s="1">
+        <v>16.112400000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>140000</v>
+      </c>
+      <c r="B159" s="1">
+        <v>14.32</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>160000</v>
+      </c>
+      <c r="B160" s="1">
+        <v>13.98</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>